<commit_message>
2025-02-18: Updated documents to reflect latest OneDrive changes (#74)
* Updating documents
---------
Authored-by: Erik <13103585+FenFideleo@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ParkingAvailabilitySystem-Documents/Meetings/TeamMeetingLog.xlsx
+++ b/ParkingAvailabilitySystem-Documents/Meetings/TeamMeetingLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/emeurrens_ufl_edu/Documents/parking-availability-system/ParkingAvailabilitySystem-Documents/Meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC11DCDE-A7CE-46B5-B62A-B583D59BB4B5}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C13CB22-D358-4A5A-8940-EFAD1165B486}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="9564" yWindow="2652" windowWidth="13824" windowHeight="7176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meeting-log" sheetId="1" r:id="rId1"/>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,6 +1224,7 @@
       <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>

</xml_diff>

<commit_message>
Updated documents to reflect final state of Beta Build
</commit_message>
<xml_diff>
--- a/ParkingAvailabilitySystem-Documents/Meetings/TeamMeetingLog.xlsx
+++ b/ParkingAvailabilitySystem-Documents/Meetings/TeamMeetingLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/emeurrens_ufl_edu/Documents/parking-availability-system/ParkingAvailabilitySystem-Documents/Meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C13CB22-D358-4A5A-8940-EFAD1165B486}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC31684A-65ED-4529-975F-2C7BB2E92CD8}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="9564" yWindow="2652" windowWidth="13824" windowHeight="7176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meeting-log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>PAS Team Meeting Log</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Stakeholder meeting with Raven discussing Alpha completion and Beta beginning. Ben got the Pi object detection model to work and communicating with the AWS backend; planning on working further on it and testing it when equipment gets here. Erik presented updates on contact with admin and materials orders. Admin hasn't given approval despite being given a January 29th deadline to respond; no response means we have plausible deniability as students to test in the garage as long as we do not interfere with the normal operation of the facility (i.e. we will test anyway). Materials to start testing are scheduled to arrive on Saturday, 9 February, and testing can begin shortly after. Erik's plans for beta are uncertain; would like to work on RPi software and object detection algorithm. The solution to the wireless network issue was discussed: current plan is to create an ESP32 repeater/network access point to bridge the gap in WiFi coverage from the UF WiFi to the location of the Raspberry Pi devices. Evan will start working on this with a goal of completing it by the end of the Beta sprint. Ryan will start working on the second iteration of the Pi housing, which aims to reduce the size of the previous housing and incorporate persistent RPi 5 power supply within it. Samer will keep working on the database and object detection model, including methods of tracking cars entering and leaving.</t>
+  </si>
+  <si>
+    <t>Stakeholder meeting discussed Beta progress. Ryan completed the second iteration of the housing, however, the 3D prints had flaws in the print and one component completely failed to print. Ben discussed progress on the Pi object detection model and current performance metrics; inference time is about 200-250 ms (4-5 fps). Goal is to reach 100 ms average. Ryan and Ben will proceed with testing the Pi on Friday. Erik completed the config script and tested USB antenna options. The config script is intended to be an evolving document that can be iterated upon. Samer worked on training the license plate recognition model. Stated that training worsened performance. Stated he has looked into the development of an administrative portal. Samer is flying to New York this weekend for an in-person job interview. Inshallah may he be safe in his travels and have success in his interview.</t>
   </si>
 </sst>
 </file>
@@ -745,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1223,8 +1226,16 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
+        <v>45707</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>

</xml_diff>

<commit_message>
Updated README to reflect work for Release Candidate. Updated documents to reflect latest changes for Release Candidate sprint.
</commit_message>
<xml_diff>
--- a/ParkingAvailabilitySystem-Documents/Meetings/TeamMeetingLog.xlsx
+++ b/ParkingAvailabilitySystem-Documents/Meetings/TeamMeetingLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/emeurrens_ufl_edu/Documents/parking-availability-system/ParkingAvailabilitySystem-Documents/Meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC31684A-65ED-4529-975F-2C7BB2E92CD8}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4A451A-441F-4BA3-9B80-CAB659E50A85}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meeting-log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>PAS Team Meeting Log</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>Stakeholder meeting discussed Beta progress. Ryan completed the second iteration of the housing, however, the 3D prints had flaws in the print and one component completely failed to print. Ben discussed progress on the Pi object detection model and current performance metrics; inference time is about 200-250 ms (4-5 fps). Goal is to reach 100 ms average. Ryan and Ben will proceed with testing the Pi on Friday. Erik completed the config script and tested USB antenna options. The config script is intended to be an evolving document that can be iterated upon. Samer worked on training the license plate recognition model. Stated that training worsened performance. Stated he has looked into the development of an administrative portal. Samer is flying to New York this weekend for an in-person job interview. Inshallah may he be safe in his travels and have success in his interview.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting to discuss Beta Presentation. Apparel most formal as possible. Trying to get a meeting time for Thursday (any time after Wednesday so we can practice our presentation with Raven). A slide for each section of the rubric (1. Context, 2. Completed Work, 3. In-Progress Work, 4. Future Work, 5. Future Plans, 6. Demo, ). Consider merging one of the slides from slides 2-4 into one and have one person present that. Live demo of system pipeline (e.g. License Plate (bring Colorado, Wyoming, or Florida plate) detected by Pi, update DB, (if time permits) show data processing through backend image pipeline, demonstrate updated counter on app). </t>
+  </si>
+  <si>
+    <t>Discussed features to work on for this sprint. Evan will continue working on ESP32 repeater until end of Spring Break; if this does not work, we will move on to a Raspberry Pi for a hotspot/repeater or look into utilizing the Sierra Airwave XT Intelligent LTE Gateway. Ryan will work on the third iteration of the housing, which may not be final, given we don't have data to work with to improve the housing. Ben will work on the camera configuration to improve camera image sharpness. Samer will do tracking, something relating to the S3 bucket and image caching, and other stuff that flew over my head. I will work on benchmark tests for hardware (temperature, frequency, and power) and possible connectivity, and hardware methods to speedup inference time (ensuring maximum core utilization, overclocking)</t>
   </si>
 </sst>
 </file>
@@ -748,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,7 +1257,16 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>45714</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1267,7 +1282,16 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>45728</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>

</xml_diff>